<commit_message>
Comparison of model to other sightlines
</commit_message>
<xml_diff>
--- a/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_185859_models_other_sightlines.xlsx
+++ b/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_185859_models_other_sightlines.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\edibles\edibles\utils\simulations\Charmi\fitting_6379_Alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F66A9A7-0D08-4478-8C8F-B06012122FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F64D0-322E-429E-9C69-027AA6FC19E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12648" yWindow="0" windowWidth="10488" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parallel_185859" sheetId="1" r:id="rId1"/>
+    <sheet name="Perpendicular_185859" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Parameters:</t>
   </si>
@@ -88,14 +89,25 @@
   </si>
   <si>
     <t>HD185859</t>
+  </si>
+  <si>
+    <t>Reduced chi square value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,16 +135,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -638,6 +657,583 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>589486</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1715699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1342899-35BE-9782-B33E-D8481D40B281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7940040" y="914400"/>
+          <a:ext cx="8514286" cy="5647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>60961</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2369820</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1682095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4362C161-13B9-7506-2241-6291023B8E0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4069081" y="746760"/>
+          <a:ext cx="2308859" cy="1666855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2377441</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1716366</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85EDFA71-654C-5022-AA01-2F15242C65C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4008121" y="2438400"/>
+          <a:ext cx="2377440" cy="1716366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45721</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2324101</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1652471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDBD443F-6D76-1278-31D5-905E1500E777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4053841" y="4236720"/>
+          <a:ext cx="2278380" cy="1644851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7621</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2278381</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1707930</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2829C5E0-28E6-7C8A-0580-EA3C61ACCCBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4015741" y="6080760"/>
+          <a:ext cx="2270760" cy="1639350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2293619</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1666447</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7364DA-A48A-B5C5-A296-5FD5FB87DF6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4046220" y="7825740"/>
+          <a:ext cx="2255519" cy="1628347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7621</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2362201</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1753203</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51E4603-FFBC-FF80-C50A-A5BAC6F11AD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4015741" y="9593580"/>
+          <a:ext cx="2354580" cy="1699863"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>45721</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2339341</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1671093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{266A4CA9-8DAD-D8D7-2542-2156E127EA56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4053841" y="11399520"/>
+          <a:ext cx="2293620" cy="1655853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>350</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1760220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00224C3B-C081-458F-5F7B-11F4D6007B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4023360" y="13136880"/>
+          <a:ext cx="2385410" cy="1722120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1671093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74CCEEBA-6CBD-54A2-E91E-6CD369A9DE3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4046221" y="15011400"/>
+          <a:ext cx="2293620" cy="1655853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2334387</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1691640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B6BDF00-2835-18DA-FA28-9C5A0F9BFBCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4030981" y="16718280"/>
+          <a:ext cx="2311526" cy="1668780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1731606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAD682B5-B2DB-9D48-508F-BB495B8153A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4030981" y="18478500"/>
+          <a:ext cx="2377440" cy="1716366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>589486</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>366959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88CE1872-FC99-B066-DB4B-5C701C9E2E8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7627620" y="731520"/>
+          <a:ext cx="8514286" cy="5647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -645,9 +1241,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}" name="Table2" displayName="Table2" ref="E5:G16" totalsRowShown="0">
   <autoFilter ref="E5:G16" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{38778A02-0510-44BD-B1B6-AF5185538A0D}" name="Sightline" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{76F21CD0-A784-4C97-83BC-E93E37DE06BF}" name="Chi-Square" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{38778A02-0510-44BD-B1B6-AF5185538A0D}" name="Sightline" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{76F21CD0-A784-4C97-83BC-E93E37DE06BF}" name="Chi-Square" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{71FF0C84-6972-423D-AB9B-6717A7985248}" name="Plot"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E8B7F7D-CE6D-4D78-A003-0DA0A2D3EB3B}" name="Table22" displayName="Table22" ref="E4:G15" totalsRowShown="0">
+  <autoFilter ref="E4:G15" xr:uid="{7E8B7F7D-CE6D-4D78-A003-0DA0A2D3EB3B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{80AEBD8C-B4DA-4C35-ACEF-6A914B5C6570}" name="Sightline" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BE7C7E3F-4A9E-4412-AB9E-369BEB296FCC}" name="Chi-Square" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{3B4F8C5F-B21F-4064-9057-901ED3DB1E00}" name="Plot"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -916,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G16"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -929,6 +1537,11 @@
     <col min="7" max="7" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
@@ -1067,6 +1680,171 @@
       </c>
       <c r="F16" s="1">
         <v>7.83967960435265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823F409E-BED1-4BED-A270-C2D15CB8042C}">
+  <dimension ref="B2:G15"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.7899999999999999E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.8802067459483194</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.8766651074412399</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>28.6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7.7602134144349204</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5.0952212277892697</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0.157</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1">
+        <v>11.406175010600601</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="145.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1">
+        <v>58.520020596606003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>66.379378978092106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="149.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11.7995862999027</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:7" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.93953188334735</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6.3502346648723602</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4.61549344503499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>